<commit_message>
se agregaron los cambios relativos en las bases
</commit_message>
<xml_diff>
--- a/Datos/pruebas random/JASP_Datos.xlsx
+++ b/Datos/pruebas random/JASP_Datos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laboratorio25_2\Desktop\Jaime_Lab25\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Jaime_Lab25\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -185,24 +185,6 @@
     <t>Subjuego</t>
   </si>
   <si>
-    <t>W1pre</t>
-  </si>
-  <si>
-    <t>W1post</t>
-  </si>
-  <si>
-    <t>W2pre</t>
-  </si>
-  <si>
-    <t>W2pos</t>
-  </si>
-  <si>
-    <t>W3pre</t>
-  </si>
-  <si>
-    <t>W3pos</t>
-  </si>
-  <si>
     <t>DO1n</t>
   </si>
   <si>
@@ -310,11 +292,29 @@
   <si>
     <t>DAP3na</t>
   </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>W5</t>
+  </si>
+  <si>
+    <t>W3_T</t>
+  </si>
+  <si>
+    <t>W2_T</t>
+  </si>
+  <si>
+    <t>W1_j1</t>
+  </si>
+  <si>
+    <t>W1_j2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,49 +1117,49 @@
         <v>37</v>
       </c>
       <c r="V1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="AC1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="AD1" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AE1" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="37" t="s">
+      <c r="AF1" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="37" t="s">
+      <c r="AG1" s="61" t="s">
         <v>64</v>
-      </c>
-      <c r="AB1" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC1" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD1" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE1" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF1" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG1" s="61" t="s">
-        <v>70</v>
       </c>
       <c r="AH1" s="51" t="s">
         <v>46</v>
       </c>
       <c r="AI1" s="51" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="AJ1" s="51" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AK1" s="51" t="s">
         <v>47</v>
@@ -1195,49 +1195,49 @@
         <v>41</v>
       </c>
       <c r="AV1" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW1" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="AX1" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY1" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ1" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA1" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB1" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="AW1" s="64" t="s">
+      <c r="BC1" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="AX1" s="64" t="s">
+      <c r="BD1" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="AY1" s="64" t="s">
+      <c r="BE1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AZ1" s="63" t="s">
+      <c r="BF1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="BA1" s="63" t="s">
+      <c r="BG1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="BB1" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="BC1" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="BD1" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="BE1" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF1" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="BG1" s="49" t="s">
-        <v>82</v>
-      </c>
       <c r="BH1" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="BI1" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="BI1" s="53" t="s">
-        <v>55</v>
-      </c>
       <c r="BJ1" s="53" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="BK1" s="53" t="s">
         <v>49</v>
@@ -1273,49 +1273,49 @@
         <v>45</v>
       </c>
       <c r="BV1" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="BW1" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX1" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY1" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="BZ1" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="CA1" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB1" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="BW1" s="65" t="s">
+      <c r="CC1" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="BX1" s="65" t="s">
+      <c r="CD1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="BY1" s="65" t="s">
+      <c r="CE1" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="BZ1" s="66" t="s">
+      <c r="CF1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="CA1" s="66" t="s">
+      <c r="CG1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="CB1" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="CC1" s="66" t="s">
+      <c r="CH1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="CI1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="CJ1" s="56" t="s">
         <v>90</v>
-      </c>
-      <c r="CD1" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="CE1" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="CF1" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="CG1" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="CH1" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="CI1" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="CJ1" s="56" t="s">
-        <v>58</v>
       </c>
       <c r="CK1" s="55" t="s">
         <v>51</v>
@@ -9417,7 +9417,7 @@
         <v>0</v>
       </c>
       <c r="AI25" s="58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ25" s="58">
         <v>1</v>
@@ -11352,7 +11352,7 @@
         <v>0</v>
       </c>
       <c r="CI30" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ30" s="59">
         <v>1</v>
@@ -11695,7 +11695,7 @@
         <v>0</v>
       </c>
       <c r="CI31" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ31" s="59">
         <v>0</v>
@@ -16298,7 +16298,7 @@
         <v>0.46190476190476198</v>
       </c>
       <c r="AH45" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI45" s="52"/>
       <c r="AJ45" s="52"/>
@@ -20837,7 +20837,7 @@
         <v>9.8039215686274536E-2</v>
       </c>
       <c r="CH58" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI58" s="45"/>
       <c r="CJ58" s="45"/>
@@ -21168,7 +21168,7 @@
         <v>0.16666666666666671</v>
       </c>
       <c r="CH59" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI59" s="45"/>
       <c r="CJ59" s="45"/>

</xml_diff>